<commit_message>
daten eingeben mit excel tabelle leicht gemacht
</commit_message>
<xml_diff>
--- a/qkd_simulation_inputs.xlsx
+++ b/qkd_simulation_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leavi\OneDrive\Dokumente\Uni\Semester 7\NeuMoQP\Programm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FCBDD1-B346-4991-A744-9460ACC78B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55451B6-1376-4A86-9890-239A42B5DF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,7 +126,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -435,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,7 +472,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D2">
         <v>0.1</v>
@@ -492,7 +492,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D3">
         <v>0.1</v>
@@ -509,7 +509,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D4">
         <v>0.1</v>
@@ -526,7 +526,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D5">
         <v>0.1</v>
@@ -543,7 +543,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D6">
         <v>0.1</v>
@@ -560,7 +560,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D7">
         <v>0.1</v>
@@ -577,7 +577,7 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D8">
         <v>0.1</v>
@@ -594,7 +594,7 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D9">
         <v>0.1</v>
@@ -611,7 +611,7 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D10">
         <v>0.11</v>
@@ -628,7 +628,7 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D11">
         <v>0.11</v>
@@ -645,7 +645,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D12">
         <v>0.11</v>
@@ -662,7 +662,7 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D13">
         <v>0.11</v>
@@ -679,7 +679,7 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D14">
         <v>0.11</v>
@@ -696,7 +696,7 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D15">
         <v>0.11</v>
@@ -713,7 +713,7 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D16">
         <v>0.11</v>
@@ -730,7 +730,7 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D17">
         <v>0.11</v>
@@ -747,7 +747,7 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D18">
         <v>0.12</v>
@@ -764,7 +764,7 @@
         <v>18</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D19">
         <v>0.12</v>
@@ -781,7 +781,7 @@
         <v>19</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D20">
         <v>0.12</v>
@@ -798,7 +798,7 @@
         <v>20</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D21">
         <v>0.12</v>
@@ -815,7 +815,7 @@
         <v>21</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D22">
         <v>0.12</v>
@@ -832,7 +832,7 @@
         <v>22</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D23">
         <v>0.12</v>
@@ -849,7 +849,7 @@
         <v>23</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D24">
         <v>0.12</v>
@@ -866,7 +866,7 @@
         <v>24</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D25">
         <v>0.12</v>
@@ -883,7 +883,7 @@
         <v>25</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D26">
         <v>0.12</v>
@@ -900,7 +900,7 @@
         <v>26</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D27">
         <v>0.13</v>
@@ -917,7 +917,7 @@
         <v>27</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D28">
         <v>0.13</v>
@@ -934,7 +934,7 @@
         <v>28</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D29">
         <v>0.13</v>
@@ -951,7 +951,7 @@
         <v>29</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D30">
         <v>0.13</v>
@@ -968,7 +968,7 @@
         <v>30</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D31">
         <v>0.13</v>
@@ -985,7 +985,7 @@
         <v>31</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D32">
         <v>0.13</v>
@@ -1002,7 +1002,7 @@
         <v>32</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D33">
         <v>0.13</v>

</xml_diff>

<commit_message>
jetzt passen die namen zusammen
</commit_message>
<xml_diff>
--- a/qkd_simulation_inputs.xlsx
+++ b/qkd_simulation_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leavi\OneDrive\Dokumente\Uni\Semester 7\NeuMoQP\Programm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55451B6-1376-4A86-9890-239A42B5DF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64CADFD-F8F0-4E9C-B6A3-5878EA521793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Run ID</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>montagnacht</t>
+  </si>
+  <si>
+    <t>dienstagmorgen</t>
   </si>
 </sst>
 </file>
@@ -433,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -994,7 +997,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>0</v>
       </c>
@@ -1009,6 +1012,361 @@
       </c>
       <c r="E33">
         <v>0.11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>-3</v>
+      </c>
+      <c r="G34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>6</v>
+      </c>
+      <c r="C39">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>9</v>
+      </c>
+      <c r="C42">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43">
+        <v>10</v>
+      </c>
+      <c r="C43">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44">
+        <v>11</v>
+      </c>
+      <c r="C44">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45">
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>13</v>
+      </c>
+      <c r="C46">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47">
+        <v>14</v>
+      </c>
+      <c r="C47">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48">
+        <v>15</v>
+      </c>
+      <c r="C48">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49">
+        <v>16</v>
+      </c>
+      <c r="C49">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <v>17</v>
+      </c>
+      <c r="C50">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <v>18</v>
+      </c>
+      <c r="C51">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>19</v>
+      </c>
+      <c r="C52">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>20</v>
+      </c>
+      <c r="C53">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>21</v>
+      </c>
+      <c r="C54">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55">
+        <v>22</v>
+      </c>
+      <c r="C55">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56">
+        <v>23</v>
+      </c>
+      <c r="C56">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57">
+        <v>24</v>
+      </c>
+      <c r="C57">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>4</v>
+      </c>
+      <c r="B58">
+        <v>25</v>
+      </c>
+      <c r="C58">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>4</v>
+      </c>
+      <c r="B59">
+        <v>26</v>
+      </c>
+      <c r="C59">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="B60">
+        <v>27</v>
+      </c>
+      <c r="C60">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>4</v>
+      </c>
+      <c r="B61">
+        <v>28</v>
+      </c>
+      <c r="C61">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>4</v>
+      </c>
+      <c r="B62">
+        <v>29</v>
+      </c>
+      <c r="C62">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>4</v>
+      </c>
+      <c r="B63">
+        <v>30</v>
+      </c>
+      <c r="C63">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>4</v>
+      </c>
+      <c r="B64">
+        <v>31</v>
+      </c>
+      <c r="C64">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>4</v>
+      </c>
+      <c r="B65">
+        <v>32</v>
+      </c>
+      <c r="C65">
+        <v>-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
umgeschrieben mit neuen files
</commit_message>
<xml_diff>
--- a/qkd_simulation_inputs.xlsx
+++ b/qkd_simulation_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leavi\OneDrive\Dokumente\Uni\Semester 7\NeuMoQP\Programm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64CADFD-F8F0-4E9C-B6A3-5878EA521793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EC0A37-BF9B-464C-BF07-2C6A1795077C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Run ID</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>dienstagmorgen</t>
+  </si>
+  <si>
+    <t>nur 25 funktioniert?</t>
   </si>
 </sst>
 </file>
@@ -436,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -503,6 +506,9 @@
       <c r="E3">
         <v>0.03</v>
       </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1022,7 +1028,13 @@
         <v>1</v>
       </c>
       <c r="C34">
-        <v>-3</v>
+        <v>-1</v>
+      </c>
+      <c r="D34">
+        <v>0.1</v>
+      </c>
+      <c r="E34">
+        <v>0.02</v>
       </c>
       <c r="G34" t="s">
         <v>7</v>
@@ -1036,7 +1048,13 @@
         <v>2</v>
       </c>
       <c r="C35">
-        <v>-3</v>
+        <v>-1</v>
+      </c>
+      <c r="D35">
+        <v>0.1</v>
+      </c>
+      <c r="E35">
+        <v>0.03</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -1047,7 +1065,13 @@
         <v>3</v>
       </c>
       <c r="C36">
-        <v>-3</v>
+        <v>-1</v>
+      </c>
+      <c r="D36">
+        <v>0.1</v>
+      </c>
+      <c r="E36">
+        <v>0.04</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -1058,7 +1082,13 @@
         <v>4</v>
       </c>
       <c r="C37">
-        <v>-3</v>
+        <v>-1</v>
+      </c>
+      <c r="D37">
+        <v>0.1</v>
+      </c>
+      <c r="E37">
+        <v>0.05</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -1069,7 +1099,13 @@
         <v>5</v>
       </c>
       <c r="C38">
-        <v>-3</v>
+        <v>-1</v>
+      </c>
+      <c r="D38">
+        <v>0.1</v>
+      </c>
+      <c r="E38">
+        <v>0.06</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -1080,29 +1116,47 @@
         <v>6</v>
       </c>
       <c r="C39">
-        <v>-3</v>
+        <v>-1</v>
+      </c>
+      <c r="D39">
+        <v>0.1</v>
+      </c>
+      <c r="E39">
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B40">
         <v>7</v>
       </c>
       <c r="C40">
-        <v>-3</v>
+        <v>-1</v>
+      </c>
+      <c r="D40">
+        <v>0.1</v>
+      </c>
+      <c r="E40">
+        <v>0.08</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B41">
         <v>8</v>
       </c>
       <c r="C41">
-        <v>-3</v>
+        <v>-1</v>
+      </c>
+      <c r="D41">
+        <v>0.1</v>
+      </c>
+      <c r="E41">
+        <v>0.09</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -1113,7 +1167,13 @@
         <v>9</v>
       </c>
       <c r="C42">
-        <v>-3</v>
+        <v>-1</v>
+      </c>
+      <c r="D42">
+        <v>0.11</v>
+      </c>
+      <c r="E42">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -1124,7 +1184,13 @@
         <v>10</v>
       </c>
       <c r="C43">
-        <v>-3</v>
+        <v>-1</v>
+      </c>
+      <c r="D43">
+        <v>0.11</v>
+      </c>
+      <c r="E43">
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -1135,7 +1201,13 @@
         <v>11</v>
       </c>
       <c r="C44">
-        <v>-3</v>
+        <v>-1</v>
+      </c>
+      <c r="D44">
+        <v>0.11</v>
+      </c>
+      <c r="E44">
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -1146,54 +1218,84 @@
         <v>12</v>
       </c>
       <c r="C45">
-        <v>-3</v>
+        <v>-1</v>
+      </c>
+      <c r="D45">
+        <v>0.11</v>
+      </c>
+      <c r="E45">
+        <v>5.5E-2</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B46">
         <v>13</v>
       </c>
       <c r="C46">
-        <v>-3</v>
+        <v>-1</v>
+      </c>
+      <c r="D46">
+        <v>0.11</v>
+      </c>
+      <c r="E46">
+        <v>6.5000000000000002E-2</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B47">
         <v>14</v>
       </c>
       <c r="C47">
-        <v>-3</v>
+        <v>-1</v>
+      </c>
+      <c r="D47">
+        <v>0.11</v>
+      </c>
+      <c r="E47">
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B48">
         <v>15</v>
       </c>
       <c r="C48">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-1</v>
+      </c>
+      <c r="D48">
+        <v>0.11</v>
+      </c>
+      <c r="E48">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B49">
         <v>16</v>
       </c>
       <c r="C49">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-1</v>
+      </c>
+      <c r="D49">
+        <v>0.11</v>
+      </c>
+      <c r="E49">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>3</v>
       </c>
@@ -1201,10 +1303,16 @@
         <v>17</v>
       </c>
       <c r="C50">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-1</v>
+      </c>
+      <c r="D50">
+        <v>0.12</v>
+      </c>
+      <c r="E50">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>3</v>
       </c>
@@ -1212,147 +1320,189 @@
         <v>18</v>
       </c>
       <c r="C51">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-1</v>
+      </c>
+      <c r="D51">
+        <v>0.12</v>
+      </c>
+      <c r="E51">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B52">
         <v>19</v>
       </c>
       <c r="C52">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-1</v>
+      </c>
+      <c r="D52">
+        <v>0.12</v>
+      </c>
+      <c r="E52">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B53">
         <v>20</v>
       </c>
       <c r="C53">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-1</v>
+      </c>
+      <c r="D53">
+        <v>0.12</v>
+      </c>
+      <c r="E53">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B54">
         <v>21</v>
       </c>
       <c r="C54">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-1</v>
+      </c>
+      <c r="D54">
+        <v>0.12</v>
+      </c>
+      <c r="E54">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B55">
         <v>22</v>
       </c>
       <c r="C55">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-1</v>
+      </c>
+      <c r="D55">
+        <v>0.12</v>
+      </c>
+      <c r="E55">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B56">
         <v>23</v>
       </c>
       <c r="C56">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-1</v>
+      </c>
+      <c r="D56">
+        <v>0.12</v>
+      </c>
+      <c r="E56">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B57">
         <v>24</v>
       </c>
       <c r="C57">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-1</v>
+      </c>
+      <c r="D57">
+        <v>0.12</v>
+      </c>
+      <c r="E57">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58">
+        <v>5</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>5</v>
+      </c>
+      <c r="B61">
         <v>4</v>
       </c>
-      <c r="B58">
-        <v>25</v>
-      </c>
-      <c r="C58">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59">
-        <v>4</v>
-      </c>
-      <c r="B59">
-        <v>26</v>
-      </c>
-      <c r="C59">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60">
-        <v>4</v>
-      </c>
-      <c r="B60">
-        <v>27</v>
-      </c>
-      <c r="C60">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61">
-        <v>4</v>
-      </c>
-      <c r="B61">
-        <v>28</v>
-      </c>
       <c r="C61">
         <v>-3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B62">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C62">
         <v>-3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B63">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C63">
         <v>-3</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B64">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C64">
         <v>-3</v>
@@ -1360,12 +1510,276 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65">
+        <v>5</v>
+      </c>
+      <c r="B65">
+        <v>8</v>
+      </c>
+      <c r="C65">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>2</v>
+      </c>
+      <c r="B66">
+        <v>9</v>
+      </c>
+      <c r="C66">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="B67">
+        <v>10</v>
+      </c>
+      <c r="C67">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="B68">
+        <v>11</v>
+      </c>
+      <c r="C68">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>2</v>
+      </c>
+      <c r="B69">
+        <v>12</v>
+      </c>
+      <c r="C69">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>2</v>
+      </c>
+      <c r="B70">
+        <v>13</v>
+      </c>
+      <c r="C70">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>2</v>
+      </c>
+      <c r="B71">
+        <v>14</v>
+      </c>
+      <c r="C71">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>2</v>
+      </c>
+      <c r="B72">
+        <v>15</v>
+      </c>
+      <c r="C72">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>2</v>
+      </c>
+      <c r="B73">
+        <v>16</v>
+      </c>
+      <c r="C73">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>3</v>
+      </c>
+      <c r="B74">
+        <v>17</v>
+      </c>
+      <c r="C74">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>3</v>
+      </c>
+      <c r="B75">
+        <v>18</v>
+      </c>
+      <c r="C75">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>3</v>
+      </c>
+      <c r="B76">
+        <v>19</v>
+      </c>
+      <c r="C76">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>3</v>
+      </c>
+      <c r="B77">
+        <v>20</v>
+      </c>
+      <c r="C77">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>3</v>
+      </c>
+      <c r="B78">
+        <v>21</v>
+      </c>
+      <c r="C78">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>3</v>
+      </c>
+      <c r="B79">
+        <v>22</v>
+      </c>
+      <c r="C79">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>3</v>
+      </c>
+      <c r="B80">
+        <v>23</v>
+      </c>
+      <c r="C80">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>3</v>
+      </c>
+      <c r="B81">
+        <v>24</v>
+      </c>
+      <c r="C81">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82">
         <v>4</v>
       </c>
-      <c r="B65">
+      <c r="B82">
+        <v>25</v>
+      </c>
+      <c r="C82">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>4</v>
+      </c>
+      <c r="B83">
+        <v>26</v>
+      </c>
+      <c r="C83">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>4</v>
+      </c>
+      <c r="B84">
+        <v>27</v>
+      </c>
+      <c r="C84">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>4</v>
+      </c>
+      <c r="B85">
+        <v>28</v>
+      </c>
+      <c r="C85">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>4</v>
+      </c>
+      <c r="B86">
+        <v>29</v>
+      </c>
+      <c r="C86">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>4</v>
+      </c>
+      <c r="B87">
+        <v>30</v>
+      </c>
+      <c r="C87">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>4</v>
+      </c>
+      <c r="B88">
+        <v>31</v>
+      </c>
+      <c r="C88">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>4</v>
+      </c>
+      <c r="B89">
         <v>32</v>
       </c>
-      <c r="C65">
+      <c r="C89">
         <v>-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
für heute abend vorbereitet
</commit_message>
<xml_diff>
--- a/qkd_simulation_inputs.xlsx
+++ b/qkd_simulation_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leavi\OneDrive\Dokumente\Uni\Semester 7\NeuMoQP\Programm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F08A6A-3FD8-4DFE-814B-F87DDD9D02E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2464A654-36A5-42B9-9698-5C01C8336C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
   <si>
     <t>Run ID</t>
   </si>
@@ -120,6 +120,27 @@
   </si>
   <si>
     <t>nicht gelaufen</t>
+  </si>
+  <si>
+    <t>läuft hoffentlich 6777853</t>
+  </si>
+  <si>
+    <t xml:space="preserve">läuft 6777850 </t>
+  </si>
+  <si>
+    <t>ab 13:00</t>
+  </si>
+  <si>
+    <t>10 Uhr Donnerstag</t>
+  </si>
+  <si>
+    <t>12 Uhr Donnerstag?</t>
+  </si>
+  <si>
+    <t>kurze runden heute abend</t>
+  </si>
+  <si>
+    <t>batches</t>
   </si>
 </sst>
 </file>
@@ -514,21 +535,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:L119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="27.7265625" customWidth="1"/>
-    <col min="7" max="7" width="64.453125" customWidth="1"/>
-    <col min="8" max="8" width="17.1796875" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="27.7265625" customWidth="1"/>
+    <col min="8" max="8" width="64.453125" customWidth="1"/>
+    <col min="9" max="9" width="17.1796875" customWidth="1"/>
+    <col min="10" max="10" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,15 +566,18 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -569,14 +593,17 @@
       <c r="E2">
         <v>0.02</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
         <v>28</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0</v>
       </c>
@@ -592,14 +619,17 @@
       <c r="E3">
         <v>0.03</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0</v>
       </c>
@@ -615,11 +645,14 @@
       <c r="E4">
         <v>0.04</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0</v>
       </c>
@@ -635,11 +668,14 @@
       <c r="E5">
         <v>0.05</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0</v>
       </c>
@@ -655,11 +691,14 @@
       <c r="E6">
         <v>0.06</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0</v>
       </c>
@@ -675,11 +714,14 @@
       <c r="E7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0</v>
       </c>
@@ -695,11 +737,14 @@
       <c r="E8">
         <v>0.08</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8">
+        <v>50</v>
+      </c>
+      <c r="G8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0</v>
       </c>
@@ -715,11 +760,14 @@
       <c r="E9">
         <v>0.09</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0</v>
       </c>
@@ -735,11 +783,14 @@
       <c r="E10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0</v>
       </c>
@@ -755,11 +806,14 @@
       <c r="E11">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0</v>
       </c>
@@ -775,11 +829,14 @@
       <c r="E12">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0</v>
       </c>
@@ -795,11 +852,14 @@
       <c r="E13">
         <v>5.5E-2</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0</v>
       </c>
@@ -815,11 +875,14 @@
       <c r="E14">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14">
+        <v>50</v>
+      </c>
+      <c r="G14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0</v>
       </c>
@@ -835,11 +898,14 @@
       <c r="E15">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0</v>
       </c>
@@ -855,11 +921,14 @@
       <c r="E16">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0</v>
       </c>
@@ -875,11 +944,14 @@
       <c r="E17">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17">
+        <v>50</v>
+      </c>
+      <c r="G17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0</v>
       </c>
@@ -895,12 +967,15 @@
       <c r="E18">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18">
+        <v>50</v>
+      </c>
+      <c r="G18" t="s">
         <v>28</v>
       </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0</v>
       </c>
@@ -916,11 +991,14 @@
       <c r="E19">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19">
+        <v>50</v>
+      </c>
+      <c r="G19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0</v>
       </c>
@@ -936,11 +1014,14 @@
       <c r="E20">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="G20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0</v>
       </c>
@@ -956,11 +1037,14 @@
       <c r="E21">
         <v>5.5E-2</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21">
+        <v>50</v>
+      </c>
+      <c r="G21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0</v>
       </c>
@@ -976,11 +1060,14 @@
       <c r="E22">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22">
+        <v>50</v>
+      </c>
+      <c r="G22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0</v>
       </c>
@@ -996,11 +1083,14 @@
       <c r="E23">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23">
+        <v>50</v>
+      </c>
+      <c r="G23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0</v>
       </c>
@@ -1016,11 +1106,14 @@
       <c r="E24">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24">
+        <v>50</v>
+      </c>
+      <c r="G24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0</v>
       </c>
@@ -1036,11 +1129,14 @@
       <c r="E25">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25">
+        <v>50</v>
+      </c>
+      <c r="G25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0</v>
       </c>
@@ -1056,15 +1152,18 @@
       <c r="E26">
         <v>0.105</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26">
+        <v>50</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1080,11 +1179,14 @@
       <c r="E27">
         <v>0.03</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27">
+        <v>50</v>
+      </c>
+      <c r="G27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0</v>
       </c>
@@ -1100,11 +1202,14 @@
       <c r="E28">
         <v>0.05</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28">
+        <v>50</v>
+      </c>
+      <c r="G28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>0</v>
       </c>
@@ -1120,11 +1225,14 @@
       <c r="E29">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29">
+        <v>50</v>
+      </c>
+      <c r="G29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>0</v>
       </c>
@@ -1140,11 +1248,14 @@
       <c r="E30">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30">
+        <v>50</v>
+      </c>
+      <c r="G30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>0</v>
       </c>
@@ -1160,15 +1271,18 @@
       <c r="E31">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31">
+        <v>50</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>0</v>
       </c>
@@ -1184,15 +1298,18 @@
       <c r="E32">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32">
+        <v>50</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>0</v>
       </c>
@@ -1208,15 +1325,18 @@
       <c r="E33">
         <v>0.11</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33">
+        <v>50</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="H33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1232,14 +1352,17 @@
       <c r="E34">
         <v>0.02</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34">
+        <v>50</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1255,11 +1378,14 @@
       <c r="E35">
         <v>0.03</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35">
+        <v>50</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1275,11 +1401,14 @@
       <c r="E36">
         <v>0.04</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36">
+        <v>50</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1295,11 +1424,14 @@
       <c r="E37">
         <v>0.05</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37">
+        <v>50</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1316,13 +1448,16 @@
         <v>0.06</v>
       </c>
       <c r="F38">
+        <v>50</v>
+      </c>
+      <c r="G38">
         <v>1124217.7522865001</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1</v>
       </c>
@@ -1338,11 +1473,14 @@
       <c r="E39">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39">
+        <v>50</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1359,13 +1497,16 @@
         <v>0.08</v>
       </c>
       <c r="F40">
+        <v>50</v>
+      </c>
+      <c r="G40">
         <v>21686397.60012088</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2</v>
       </c>
@@ -1382,13 +1523,16 @@
         <v>0.09</v>
       </c>
       <c r="F41">
+        <v>50</v>
+      </c>
+      <c r="G41">
         <v>37829581.426437467</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1404,11 +1548,14 @@
       <c r="E42">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42">
+        <v>50</v>
+      </c>
+      <c r="G42" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2</v>
       </c>
@@ -1424,11 +1571,14 @@
       <c r="E43">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43">
+        <v>50</v>
+      </c>
+      <c r="G43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1444,11 +1594,14 @@
       <c r="E44">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44">
+        <v>50</v>
+      </c>
+      <c r="G44" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1464,11 +1617,14 @@
       <c r="E45">
         <v>5.5E-2</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45">
+        <v>50</v>
+      </c>
+      <c r="G45" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>3</v>
       </c>
@@ -1485,13 +1641,16 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F46">
+        <v>50</v>
+      </c>
+      <c r="G46">
         <v>88665.890940519996</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>3</v>
       </c>
@@ -1508,13 +1667,16 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="F47">
+        <v>50</v>
+      </c>
+      <c r="G47">
         <v>10937284.017534729</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>3</v>
       </c>
@@ -1531,13 +1693,16 @@
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="F48">
+        <v>50</v>
+      </c>
+      <c r="G48">
         <v>21835719.924602289</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>3</v>
       </c>
@@ -1554,13 +1719,16 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="F49">
+        <v>50</v>
+      </c>
+      <c r="G49">
         <v>35086121.701041572</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>3</v>
       </c>
@@ -1576,11 +1744,14 @@
       <c r="E50">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50">
+        <v>50</v>
+      </c>
+      <c r="G50" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>3</v>
       </c>
@@ -1596,11 +1767,14 @@
       <c r="E51">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51">
+        <v>50</v>
+      </c>
+      <c r="G51" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>4</v>
       </c>
@@ -1616,11 +1790,14 @@
       <c r="E52">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52">
+        <v>50</v>
+      </c>
+      <c r="G52" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>4</v>
       </c>
@@ -1636,11 +1813,14 @@
       <c r="E53">
         <v>5.5E-2</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53">
+        <v>50</v>
+      </c>
+      <c r="G53" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>4</v>
       </c>
@@ -1656,11 +1836,14 @@
       <c r="E54">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54">
+        <v>50</v>
+      </c>
+      <c r="G54" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>4</v>
       </c>
@@ -1676,11 +1859,14 @@
       <c r="E55">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55">
+        <v>50</v>
+      </c>
+      <c r="G55" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>4</v>
       </c>
@@ -1697,13 +1883,16 @@
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="F56">
+        <v>50</v>
+      </c>
+      <c r="G56">
         <v>3627593.6092775399</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>4</v>
       </c>
@@ -1720,13 +1909,16 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="F57">
+        <v>50</v>
+      </c>
+      <c r="G57">
         <v>16363177.18720264</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>5</v>
       </c>
@@ -1742,8 +1934,11 @@
       <c r="E58">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F58">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>5</v>
       </c>
@@ -1759,8 +1954,11 @@
       <c r="E59">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F59">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>5</v>
       </c>
@@ -1776,8 +1974,11 @@
       <c r="E60">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F60">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>5</v>
       </c>
@@ -1793,8 +1994,11 @@
       <c r="E61">
         <v>5.5E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F61">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>5</v>
       </c>
@@ -1810,8 +2014,11 @@
       <c r="E62">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F62">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>5</v>
       </c>
@@ -1827,8 +2034,11 @@
       <c r="E63">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F63">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>5</v>
       </c>
@@ -1844,8 +2054,11 @@
       <c r="E64">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F64">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>5</v>
       </c>
@@ -1861,8 +2074,11 @@
       <c r="E65">
         <v>3.5000000000000003E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F65">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>6</v>
       </c>
@@ -1878,8 +2094,11 @@
       <c r="E66">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F66">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>6</v>
       </c>
@@ -1895,8 +2114,11 @@
       <c r="E67">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F67">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>6</v>
       </c>
@@ -1912,8 +2134,11 @@
       <c r="E68">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F68">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>6</v>
       </c>
@@ -1929,8 +2154,11 @@
       <c r="E69">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F69">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>6</v>
       </c>
@@ -1946,8 +2174,11 @@
       <c r="E70">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F70">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>6</v>
       </c>
@@ -1963,8 +2194,11 @@
       <c r="E71">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F71">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>6</v>
       </c>
@@ -1980,8 +2214,11 @@
       <c r="E72">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F72">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>6</v>
       </c>
@@ -1997,8 +2234,11 @@
       <c r="E73">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F73">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>7</v>
       </c>
@@ -2014,8 +2254,11 @@
       <c r="E74">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F74">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>7</v>
       </c>
@@ -2031,8 +2274,11 @@
       <c r="E75">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F75">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>7</v>
       </c>
@@ -2048,8 +2294,11 @@
       <c r="E76">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F76">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>7</v>
       </c>
@@ -2065,8 +2314,11 @@
       <c r="E77">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F77">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>7</v>
       </c>
@@ -2082,8 +2334,11 @@
       <c r="E78">
         <v>9.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F78">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>7</v>
       </c>
@@ -2099,8 +2354,11 @@
       <c r="E79">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F79">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>7</v>
       </c>
@@ -2116,8 +2374,11 @@
       <c r="E80">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F80">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>7</v>
       </c>
@@ -2133,8 +2394,11 @@
       <c r="E81">
         <v>0.14499999999999999</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F81">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>8</v>
       </c>
@@ -2150,8 +2414,11 @@
       <c r="E82">
         <v>0.155</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F82">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>8</v>
       </c>
@@ -2167,8 +2434,11 @@
       <c r="E83">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F83">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>8</v>
       </c>
@@ -2184,8 +2454,11 @@
       <c r="E84">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F84">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>8</v>
       </c>
@@ -2201,8 +2474,11 @@
       <c r="E85">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F85">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>8</v>
       </c>
@@ -2218,8 +2494,11 @@
       <c r="E86">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F86">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>8</v>
       </c>
@@ -2235,8 +2514,11 @@
       <c r="E87">
         <v>0.14499999999999999</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F87">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>8</v>
       </c>
@@ -2252,8 +2534,11 @@
       <c r="E88">
         <v>0.155</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F88">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>8</v>
       </c>
@@ -2269,8 +2554,11 @@
       <c r="E89">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F89">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>9</v>
       </c>
@@ -2286,8 +2574,17 @@
       <c r="E90">
         <v>0.215</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F90">
+        <v>50</v>
+      </c>
+      <c r="J90" t="s">
+        <v>29</v>
+      </c>
+      <c r="L90" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>9</v>
       </c>
@@ -2303,8 +2600,11 @@
       <c r="E91">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F91">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>9</v>
       </c>
@@ -2320,8 +2620,11 @@
       <c r="E92">
         <v>0.245</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F92">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>9</v>
       </c>
@@ -2337,8 +2640,11 @@
       <c r="E93">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F93">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>9</v>
       </c>
@@ -2354,8 +2660,11 @@
       <c r="E94">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F94">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>9</v>
       </c>
@@ -2371,8 +2680,11 @@
       <c r="E95">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F95">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>9</v>
       </c>
@@ -2386,14 +2698,17 @@
         <v>0.45</v>
       </c>
       <c r="E96">
-        <f>D96*H96</f>
+        <f>D96*I96</f>
         <v>0.315</v>
       </c>
-      <c r="H96">
+      <c r="F96">
+        <v>50</v>
+      </c>
+      <c r="I96">
         <v>0.7</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>9</v>
       </c>
@@ -2409,8 +2724,11 @@
       <c r="E97">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F97">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>9</v>
       </c>
@@ -2426,8 +2744,11 @@
       <c r="E98">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F98">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>9</v>
       </c>
@@ -2441,14 +2762,17 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="E99">
-        <f>D99*H99</f>
+        <f>D99*I99</f>
         <v>0.38500000000000001</v>
       </c>
-      <c r="H99">
+      <c r="F99">
+        <v>50</v>
+      </c>
+      <c r="I99">
         <v>0.7</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>9</v>
       </c>
@@ -2464,8 +2788,11 @@
       <c r="E100">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F100">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>9</v>
       </c>
@@ -2481,8 +2808,11 @@
       <c r="E101">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F101">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>10</v>
       </c>
@@ -2498,8 +2828,20 @@
       <c r="E102">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F102">
+        <v>50</v>
+      </c>
+      <c r="J102" t="s">
+        <v>30</v>
+      </c>
+      <c r="K102" t="s">
+        <v>31</v>
+      </c>
+      <c r="L102" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>10</v>
       </c>
@@ -2513,14 +2855,17 @@
         <v>0.75</v>
       </c>
       <c r="E103">
-        <f>D103*H103</f>
+        <f>D103*I103</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="H103">
+      <c r="F103">
+        <v>50</v>
+      </c>
+      <c r="I103">
         <v>0.8</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>10</v>
       </c>
@@ -2536,8 +2881,11 @@
       <c r="E104">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F104">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>10</v>
       </c>
@@ -2553,8 +2901,11 @@
       <c r="E105">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F105">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>10</v>
       </c>
@@ -2570,8 +2921,11 @@
       <c r="E106">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F106">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>10</v>
       </c>
@@ -2587,8 +2941,11 @@
       <c r="E107">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F107">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>10</v>
       </c>
@@ -2604,8 +2961,11 @@
       <c r="E108">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F108">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>10</v>
       </c>
@@ -2621,8 +2981,11 @@
       <c r="E109">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F109">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>10</v>
       </c>
@@ -2638,8 +3001,11 @@
       <c r="E110">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F110">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>10</v>
       </c>
@@ -2655,8 +3021,11 @@
       <c r="E111">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F111">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>10</v>
       </c>
@@ -2672,8 +3041,11 @@
       <c r="E112">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F112">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>10</v>
       </c>
@@ -2688,6 +3060,156 @@
       </c>
       <c r="E113">
         <v>0.65</v>
+      </c>
+      <c r="F113">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>11</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="C114">
+        <v>-12</v>
+      </c>
+      <c r="D114">
+        <v>0.65</v>
+      </c>
+      <c r="E114">
+        <f>D114*I114</f>
+        <v>0.45499999999999996</v>
+      </c>
+      <c r="F114">
+        <v>100</v>
+      </c>
+      <c r="I114">
+        <v>0.7</v>
+      </c>
+      <c r="J114" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>11</v>
+      </c>
+      <c r="B115">
+        <v>2</v>
+      </c>
+      <c r="C115">
+        <v>-12</v>
+      </c>
+      <c r="D115">
+        <v>0.65</v>
+      </c>
+      <c r="E115">
+        <f>D115*I115</f>
+        <v>0.52</v>
+      </c>
+      <c r="F115">
+        <v>100</v>
+      </c>
+      <c r="I115">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>11</v>
+      </c>
+      <c r="B116">
+        <v>3</v>
+      </c>
+      <c r="C116">
+        <v>-12</v>
+      </c>
+      <c r="D116">
+        <v>0.65</v>
+      </c>
+      <c r="E116">
+        <f t="shared" ref="E115:E119" si="0">D116*I116</f>
+        <v>0.58500000000000008</v>
+      </c>
+      <c r="F116">
+        <v>100</v>
+      </c>
+      <c r="I116">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>12</v>
+      </c>
+      <c r="B117">
+        <v>4</v>
+      </c>
+      <c r="C117">
+        <v>-12</v>
+      </c>
+      <c r="D117">
+        <v>0.7</v>
+      </c>
+      <c r="E117">
+        <f t="shared" si="0"/>
+        <v>0.48999999999999994</v>
+      </c>
+      <c r="F117">
+        <v>100</v>
+      </c>
+      <c r="I117">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>12</v>
+      </c>
+      <c r="B118">
+        <v>5</v>
+      </c>
+      <c r="C118">
+        <v>-12</v>
+      </c>
+      <c r="D118">
+        <v>0.7</v>
+      </c>
+      <c r="E118">
+        <f t="shared" si="0"/>
+        <v>0.55999999999999994</v>
+      </c>
+      <c r="F118">
+        <v>100</v>
+      </c>
+      <c r="I118">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>12</v>
+      </c>
+      <c r="B119">
+        <v>6</v>
+      </c>
+      <c r="C119">
+        <v>-12</v>
+      </c>
+      <c r="D119">
+        <v>0.7</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="0"/>
+        <v>0.63</v>
+      </c>
+      <c r="F119">
+        <v>100</v>
+      </c>
+      <c r="I119">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
neue daten in tabelle
</commit_message>
<xml_diff>
--- a/qkd_simulation_inputs.xlsx
+++ b/qkd_simulation_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leavi\OneDrive\Dokumente\Uni\Semester 7\NeuMoQP\Programm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC113C25-33F4-476B-9441-3F7F14AB812A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996FAB3F-3609-4ECD-8788-39C4A26DE316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -710,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L173"/>
+  <dimension ref="A1:L221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="G120" sqref="G120"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="G221" sqref="G221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5040,6 +5040,968 @@
         <v>0.95</v>
       </c>
     </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A174">
+        <v>22</v>
+      </c>
+      <c r="B174">
+        <v>1</v>
+      </c>
+      <c r="C174">
+        <v>-1</v>
+      </c>
+      <c r="D174">
+        <v>0.13</v>
+      </c>
+      <c r="E174">
+        <v>0.12</v>
+      </c>
+      <c r="F174">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A175">
+        <v>22</v>
+      </c>
+      <c r="B175">
+        <v>2</v>
+      </c>
+      <c r="C175">
+        <v>-1</v>
+      </c>
+      <c r="D175">
+        <v>0.13</v>
+      </c>
+      <c r="E175">
+        <v>0.125</v>
+      </c>
+      <c r="F175">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A176">
+        <v>22</v>
+      </c>
+      <c r="B176">
+        <v>3</v>
+      </c>
+      <c r="C176">
+        <v>-1</v>
+      </c>
+      <c r="D176">
+        <v>0.1</v>
+      </c>
+      <c r="E176">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F176">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A177">
+        <v>22</v>
+      </c>
+      <c r="B177">
+        <v>4</v>
+      </c>
+      <c r="C177">
+        <v>-1</v>
+      </c>
+      <c r="D177">
+        <v>0.11</v>
+      </c>
+      <c r="E177">
+        <v>5.5E-2</v>
+      </c>
+      <c r="F177">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A178">
+        <v>22</v>
+      </c>
+      <c r="B178">
+        <v>5</v>
+      </c>
+      <c r="C178">
+        <v>-3</v>
+      </c>
+      <c r="D178">
+        <v>0.125</v>
+      </c>
+      <c r="E178">
+        <v>0.09</v>
+      </c>
+      <c r="F178">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A179">
+        <v>22</v>
+      </c>
+      <c r="B179">
+        <v>6</v>
+      </c>
+      <c r="C179">
+        <v>-3</v>
+      </c>
+      <c r="D179">
+        <v>0.125</v>
+      </c>
+      <c r="E179">
+        <v>0.11</v>
+      </c>
+      <c r="F179">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A180">
+        <v>23</v>
+      </c>
+      <c r="B180">
+        <v>7</v>
+      </c>
+      <c r="C180">
+        <v>-3</v>
+      </c>
+      <c r="D180">
+        <v>0.125</v>
+      </c>
+      <c r="E180">
+        <v>0.12</v>
+      </c>
+      <c r="F180">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A181">
+        <v>23</v>
+      </c>
+      <c r="B181">
+        <v>8</v>
+      </c>
+      <c r="C181">
+        <v>-1</v>
+      </c>
+      <c r="D181">
+        <v>0.12</v>
+      </c>
+      <c r="E181">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F181">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A182">
+        <v>23</v>
+      </c>
+      <c r="B182">
+        <v>9</v>
+      </c>
+      <c r="C182">
+        <v>-3</v>
+      </c>
+      <c r="D182">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="E182">
+        <v>0.09</v>
+      </c>
+      <c r="F182">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A183">
+        <v>23</v>
+      </c>
+      <c r="B183">
+        <v>10</v>
+      </c>
+      <c r="C183">
+        <v>-3</v>
+      </c>
+      <c r="D183">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="E183">
+        <v>0.11</v>
+      </c>
+      <c r="F183">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A184">
+        <v>23</v>
+      </c>
+      <c r="B184">
+        <v>11</v>
+      </c>
+      <c r="C184">
+        <v>-3</v>
+      </c>
+      <c r="D184">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="E184">
+        <v>0.13</v>
+      </c>
+      <c r="F184">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A185">
+        <v>23</v>
+      </c>
+      <c r="B185">
+        <v>12</v>
+      </c>
+      <c r="C185">
+        <v>-3</v>
+      </c>
+      <c r="D185">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="E185">
+        <v>0.08</v>
+      </c>
+      <c r="F185">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A186">
+        <v>24</v>
+      </c>
+      <c r="B186">
+        <v>13</v>
+      </c>
+      <c r="C186">
+        <v>-3</v>
+      </c>
+      <c r="D186">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="E186">
+        <v>0.1</v>
+      </c>
+      <c r="F186">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A187">
+        <v>24</v>
+      </c>
+      <c r="B187">
+        <v>14</v>
+      </c>
+      <c r="C187">
+        <v>-3</v>
+      </c>
+      <c r="D187">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="E187">
+        <v>0.12</v>
+      </c>
+      <c r="F187">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A188">
+        <v>24</v>
+      </c>
+      <c r="B188">
+        <v>15</v>
+      </c>
+      <c r="C188">
+        <v>-3</v>
+      </c>
+      <c r="D188">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="E188">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F188">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A189">
+        <v>24</v>
+      </c>
+      <c r="B189">
+        <v>16</v>
+      </c>
+      <c r="C189">
+        <v>-3</v>
+      </c>
+      <c r="D189">
+        <v>0.155</v>
+      </c>
+      <c r="E189">
+        <v>0.08</v>
+      </c>
+      <c r="F189">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A190">
+        <v>24</v>
+      </c>
+      <c r="B190">
+        <v>17</v>
+      </c>
+      <c r="C190">
+        <v>-3</v>
+      </c>
+      <c r="D190">
+        <v>0.155</v>
+      </c>
+      <c r="E190">
+        <v>0.1</v>
+      </c>
+      <c r="F190">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A191">
+        <v>24</v>
+      </c>
+      <c r="B191">
+        <v>18</v>
+      </c>
+      <c r="C191">
+        <v>-3</v>
+      </c>
+      <c r="D191">
+        <v>0.155</v>
+      </c>
+      <c r="E191">
+        <v>0.12</v>
+      </c>
+      <c r="F191">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A192">
+        <v>25</v>
+      </c>
+      <c r="B192">
+        <v>19</v>
+      </c>
+      <c r="C192">
+        <v>-3</v>
+      </c>
+      <c r="D192">
+        <v>0.155</v>
+      </c>
+      <c r="E192">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F192">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A193">
+        <v>25</v>
+      </c>
+      <c r="B193">
+        <v>20</v>
+      </c>
+      <c r="C193">
+        <v>-3</v>
+      </c>
+      <c r="D193">
+        <v>0.155</v>
+      </c>
+      <c r="E193">
+        <v>0.15</v>
+      </c>
+      <c r="F193">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A194">
+        <v>25</v>
+      </c>
+      <c r="B194">
+        <v>21</v>
+      </c>
+      <c r="C194">
+        <v>-1</v>
+      </c>
+      <c r="D194">
+        <v>0.12</v>
+      </c>
+      <c r="E194">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="F194">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A195">
+        <v>25</v>
+      </c>
+      <c r="B195">
+        <v>22</v>
+      </c>
+      <c r="C195">
+        <v>-3</v>
+      </c>
+      <c r="D195">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="E195">
+        <v>0.11</v>
+      </c>
+      <c r="F195">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A196">
+        <v>25</v>
+      </c>
+      <c r="B196">
+        <v>23</v>
+      </c>
+      <c r="C196">
+        <v>-3</v>
+      </c>
+      <c r="D196">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="E196">
+        <v>0.13</v>
+      </c>
+      <c r="F196">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A197">
+        <v>25</v>
+      </c>
+      <c r="B197">
+        <v>24</v>
+      </c>
+      <c r="C197">
+        <v>-3</v>
+      </c>
+      <c r="D197">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="E197">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="F197">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A198">
+        <v>26</v>
+      </c>
+      <c r="B198">
+        <v>25</v>
+      </c>
+      <c r="C198">
+        <v>-3</v>
+      </c>
+      <c r="D198">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="E198">
+        <v>0.155</v>
+      </c>
+      <c r="F198">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A199">
+        <v>26</v>
+      </c>
+      <c r="B199">
+        <v>26</v>
+      </c>
+      <c r="C199">
+        <v>-3</v>
+      </c>
+      <c r="D199">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="E199">
+        <v>0.16</v>
+      </c>
+      <c r="F199">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A200">
+        <v>26</v>
+      </c>
+      <c r="B200">
+        <v>27</v>
+      </c>
+      <c r="C200">
+        <v>-3</v>
+      </c>
+      <c r="D200">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E200">
+        <v>0.09</v>
+      </c>
+      <c r="F200">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A201">
+        <v>26</v>
+      </c>
+      <c r="B201">
+        <v>28</v>
+      </c>
+      <c r="C201">
+        <v>-3</v>
+      </c>
+      <c r="D201">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E201">
+        <v>0.11</v>
+      </c>
+      <c r="F201">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A202">
+        <v>26</v>
+      </c>
+      <c r="B202">
+        <v>29</v>
+      </c>
+      <c r="C202">
+        <v>-3</v>
+      </c>
+      <c r="D202">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E202">
+        <v>0.13</v>
+      </c>
+      <c r="F202">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A203">
+        <v>26</v>
+      </c>
+      <c r="B203">
+        <v>30</v>
+      </c>
+      <c r="C203">
+        <v>-3</v>
+      </c>
+      <c r="D203">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E203">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="F203">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A204">
+        <v>27</v>
+      </c>
+      <c r="B204">
+        <v>31</v>
+      </c>
+      <c r="C204">
+        <v>-3</v>
+      </c>
+      <c r="D204">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E204">
+        <v>0.155</v>
+      </c>
+      <c r="F204">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A205">
+        <v>27</v>
+      </c>
+      <c r="B205">
+        <v>32</v>
+      </c>
+      <c r="C205">
+        <v>-3</v>
+      </c>
+      <c r="D205">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E205">
+        <v>0.16</v>
+      </c>
+      <c r="F205">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A206">
+        <v>27</v>
+      </c>
+      <c r="B206">
+        <v>33</v>
+      </c>
+      <c r="C206">
+        <v>-6</v>
+      </c>
+      <c r="D206">
+        <v>0.35</v>
+      </c>
+      <c r="E206">
+        <v>0.33</v>
+      </c>
+      <c r="F206">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A207">
+        <v>27</v>
+      </c>
+      <c r="B207">
+        <v>34</v>
+      </c>
+      <c r="C207">
+        <v>-6</v>
+      </c>
+      <c r="D207">
+        <v>0.45</v>
+      </c>
+      <c r="E207">
+        <f>D207*I207</f>
+        <v>0</v>
+      </c>
+      <c r="F207">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A208">
+        <v>27</v>
+      </c>
+      <c r="B208">
+        <v>35</v>
+      </c>
+      <c r="C208">
+        <v>-6</v>
+      </c>
+      <c r="D208">
+        <v>0.45</v>
+      </c>
+      <c r="E208">
+        <v>0.38</v>
+      </c>
+      <c r="F208">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A209">
+        <v>27</v>
+      </c>
+      <c r="B209">
+        <v>36</v>
+      </c>
+      <c r="C209">
+        <v>-6</v>
+      </c>
+      <c r="D209">
+        <v>0.45</v>
+      </c>
+      <c r="E209">
+        <v>0.42</v>
+      </c>
+      <c r="F209">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A210">
+        <v>28</v>
+      </c>
+      <c r="B210">
+        <v>37</v>
+      </c>
+      <c r="C210">
+        <v>-6</v>
+      </c>
+      <c r="D210">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E210">
+        <f>D210*I210</f>
+        <v>0</v>
+      </c>
+      <c r="F210">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A211">
+        <v>28</v>
+      </c>
+      <c r="B211">
+        <v>38</v>
+      </c>
+      <c r="C211">
+        <v>-6</v>
+      </c>
+      <c r="D211">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E211">
+        <v>0.44</v>
+      </c>
+      <c r="F211">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A212">
+        <v>28</v>
+      </c>
+      <c r="B212">
+        <v>39</v>
+      </c>
+      <c r="C212">
+        <v>-6</v>
+      </c>
+      <c r="D212">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E212">
+        <v>0.5</v>
+      </c>
+      <c r="F212">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A213">
+        <v>28</v>
+      </c>
+      <c r="B213">
+        <v>40</v>
+      </c>
+      <c r="C213">
+        <v>-6</v>
+      </c>
+      <c r="D213">
+        <v>0.65</v>
+      </c>
+      <c r="E213">
+        <v>0.53</v>
+      </c>
+      <c r="F213">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A214">
+        <v>28</v>
+      </c>
+      <c r="B214">
+        <v>41</v>
+      </c>
+      <c r="C214">
+        <v>-9</v>
+      </c>
+      <c r="D214">
+        <v>0.5</v>
+      </c>
+      <c r="E214">
+        <v>0.47</v>
+      </c>
+      <c r="F214">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A215">
+        <v>28</v>
+      </c>
+      <c r="B215">
+        <v>42</v>
+      </c>
+      <c r="C215">
+        <v>-9</v>
+      </c>
+      <c r="D215">
+        <v>0.6</v>
+      </c>
+      <c r="E215">
+        <v>0.45</v>
+      </c>
+      <c r="F215">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A216">
+        <v>29</v>
+      </c>
+      <c r="B216">
+        <v>43</v>
+      </c>
+      <c r="C216">
+        <v>-9</v>
+      </c>
+      <c r="D216">
+        <v>0.6</v>
+      </c>
+      <c r="E216">
+        <v>0.5</v>
+      </c>
+      <c r="F216">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A217">
+        <v>29</v>
+      </c>
+      <c r="B217">
+        <v>44</v>
+      </c>
+      <c r="C217">
+        <v>-9</v>
+      </c>
+      <c r="D217">
+        <v>0.6</v>
+      </c>
+      <c r="E217">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F217">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A218">
+        <v>29</v>
+      </c>
+      <c r="B218">
+        <v>45</v>
+      </c>
+      <c r="C218">
+        <v>-9</v>
+      </c>
+      <c r="D218">
+        <v>0.7</v>
+      </c>
+      <c r="E218">
+        <v>0.45</v>
+      </c>
+      <c r="F218">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A219">
+        <v>29</v>
+      </c>
+      <c r="B219">
+        <v>46</v>
+      </c>
+      <c r="C219">
+        <v>-9</v>
+      </c>
+      <c r="D219">
+        <v>0.7</v>
+      </c>
+      <c r="E219">
+        <v>0.5</v>
+      </c>
+      <c r="F219">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A220">
+        <v>29</v>
+      </c>
+      <c r="B220">
+        <v>47</v>
+      </c>
+      <c r="C220">
+        <v>-9</v>
+      </c>
+      <c r="D220">
+        <v>0.7</v>
+      </c>
+      <c r="E220">
+        <v>0.6</v>
+      </c>
+      <c r="F220">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A221">
+        <v>29</v>
+      </c>
+      <c r="B221">
+        <v>48</v>
+      </c>
+      <c r="C221">
+        <v>-9</v>
+      </c>
+      <c r="D221">
+        <v>0.7</v>
+      </c>
+      <c r="E221">
+        <v>0.65</v>
+      </c>
+      <c r="F221">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>